<commit_message>
FinalPractice: Ending with the proposal of the logic
</commit_message>
<xml_diff>
--- a/Working with Tables in Excel/Data/CardPayments.xlsx
+++ b/Working with Tables in Excel/Data/CardPayments.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0372D330-4CA0-458C-B46B-5D5EE48A60EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3050E0-EBE9-4838-9D7B-BA3CD75B55EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,11 +412,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>

</xml_diff>